<commit_message>
chore(so): update system templates
</commit_message>
<xml_diff>
--- a/document-merge-service/kt_so/templatefiles/pruefung-kanalisationsanschluss-und-versickerungsanlage.xlsx
+++ b/document-merge-service/kt_so/templatefiles/pruefung-kanalisationsanschluss-und-versickerungsanlage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\BJSVW\Agi\eBau\Dokumentenvorlagen\eBau\Systemvorlagen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72BAC62-7673-4EB3-9A6A-8BF12EA67B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E01795-19AA-46E4-B13C-7C4E5CB5EB15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="645" windowWidth="25200" windowHeight="14835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2175" yWindow="210" windowWidth="27015" windowHeight="15045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vorprüfung gross" sheetId="1" r:id="rId1"/>
@@ -1030,21 +1030,6 @@
   </si>
   <si>
     <t>Wegbreite</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dossier-Nr.: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>{{ DOSSIER_NUMMER }}</t>
-    </r>
   </si>
   <si>
     <t>{{ BESCHREIBUNG_BAUVORHABEN }}</t>
@@ -1102,6 +1087,9 @@
     <t>{{ ALLE_GESUCHSTELLER_NAME_ADRESSE }}</t>
   </si>
   <si>
+    <t>Dossier-Nr.: {{ DOSSIER_NUMMER }}</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Grundstücksnummer: </t>
     </r>
@@ -1109,7 +1097,6 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FF00B050"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -1125,7 +1112,6 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FF00B050"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -1140,7 +1126,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ &quot;SFr.&quot;\ * #,##0.00_ ;_ &quot;SFr.&quot;\ * \-#,##0.00_ ;_ &quot;SFr.&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1266,20 +1252,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF00B050"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color rgb="FF00B050"/>
       <name val="Arial"/>
@@ -1287,16 +1259,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF00B050"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1634,7 +1599,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="247">
+  <cellXfs count="249">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2154,196 +2119,204 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2629,8 +2602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L344"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2646,26 +2619,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="186" t="s">
-        <v>266</v>
+      <c r="A1" s="17" t="s">
+        <v>265</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="187"/>
+      <c r="J1" s="184"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="188" t="s">
-        <v>267</v>
+      <c r="A2" s="237" t="s">
+        <v>266</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
       <c r="E2"/>
       <c r="F2"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="189"/>
+      <c r="J2" s="185"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I3" s="3"/>
@@ -2699,68 +2672,68 @@
     </row>
     <row r="6" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="B6" s="211" t="s">
+        <v>264</v>
+      </c>
+      <c r="B6" s="238" t="s">
+        <v>267</v>
+      </c>
+      <c r="C6" s="239"/>
+      <c r="D6" s="239"/>
+      <c r="E6" s="239"/>
+      <c r="F6" s="239"/>
+      <c r="G6" s="239"/>
+      <c r="H6" s="239"/>
+      <c r="I6" s="240"/>
+      <c r="J6" s="11" t="s">
         <v>268</v>
-      </c>
-      <c r="C6" s="212"/>
-      <c r="D6" s="212"/>
-      <c r="E6" s="212"/>
-      <c r="F6" s="212"/>
-      <c r="G6" s="212"/>
-      <c r="H6" s="212"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="11" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="213" t="s">
-        <v>259</v>
-      </c>
-      <c r="C7" s="214"/>
-      <c r="D7" s="214"/>
-      <c r="E7" s="214"/>
-      <c r="F7" s="214"/>
-      <c r="G7" s="214"/>
-      <c r="H7" s="214"/>
-      <c r="I7" s="214"/>
+      <c r="B7" s="241" t="s">
+        <v>258</v>
+      </c>
+      <c r="C7" s="242"/>
+      <c r="D7" s="242"/>
+      <c r="E7" s="242"/>
+      <c r="F7" s="242"/>
+      <c r="G7" s="242"/>
+      <c r="H7" s="242"/>
+      <c r="I7" s="242"/>
       <c r="J7" s="13"/>
     </row>
     <row r="8" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="213" t="s">
-        <v>260</v>
-      </c>
-      <c r="C8" s="215"/>
-      <c r="D8" s="215"/>
-      <c r="E8" s="215"/>
-      <c r="F8" s="215"/>
-      <c r="G8" s="215"/>
-      <c r="H8" s="215"/>
-      <c r="I8" s="215"/>
+      <c r="B8" s="241" t="s">
+        <v>259</v>
+      </c>
+      <c r="C8" s="243"/>
+      <c r="D8" s="243"/>
+      <c r="E8" s="243"/>
+      <c r="F8" s="243"/>
+      <c r="G8" s="243"/>
+      <c r="H8" s="243"/>
+      <c r="I8" s="243"/>
       <c r="J8" s="13"/>
     </row>
     <row r="9" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="180" t="s">
+        <v>260</v>
+      </c>
+      <c r="B9" s="244" t="s">
         <v>261</v>
       </c>
-      <c r="B9" s="181" t="s">
-        <v>262</v>
-      </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
+      <c r="C9" s="245"/>
+      <c r="D9" s="245"/>
+      <c r="E9" s="245"/>
+      <c r="F9" s="245"/>
+      <c r="G9" s="245"/>
+      <c r="H9" s="246"/>
+      <c r="I9" s="246"/>
       <c r="J9" s="13"/>
     </row>
     <row r="10" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2840,35 +2813,35 @@
       <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="216" t="s">
+      <c r="A16" s="186" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="218" t="s">
+      <c r="B16" s="188" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="220" t="s">
+      <c r="C16" s="190" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="222" t="s">
+      <c r="D16" s="192" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="223"/>
-      <c r="F16" s="224"/>
-      <c r="G16" s="222" t="s">
+      <c r="E16" s="193"/>
+      <c r="F16" s="194"/>
+      <c r="G16" s="192" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="223"/>
-      <c r="I16" s="224"/>
-      <c r="J16" s="199" t="s">
+      <c r="H16" s="193"/>
+      <c r="I16" s="194"/>
+      <c r="J16" s="198" t="s">
         <v>10</v>
       </c>
-      <c r="K16" s="201"/>
-      <c r="L16" s="201"/>
+      <c r="K16" s="200"/>
+      <c r="L16" s="200"/>
     </row>
     <row r="17" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="217"/>
-      <c r="B17" s="219"/>
-      <c r="C17" s="221"/>
+      <c r="A17" s="187"/>
+      <c r="B17" s="189"/>
+      <c r="C17" s="191"/>
       <c r="D17" s="18" t="s">
         <v>11</v>
       </c>
@@ -2887,9 +2860,9 @@
       <c r="I17" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="J17" s="200"/>
-      <c r="K17" s="201"/>
-      <c r="L17" s="201"/>
+      <c r="J17" s="199"/>
+      <c r="K17" s="200"/>
+      <c r="L17" s="200"/>
     </row>
     <row r="18" spans="1:12" s="23" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
@@ -3475,28 +3448,28 @@
       <c r="I46" s="42"/>
     </row>
     <row r="47" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="202"/>
-      <c r="B47" s="203"/>
-      <c r="C47" s="203"/>
-      <c r="D47" s="203"/>
-      <c r="E47" s="203"/>
-      <c r="F47" s="203"/>
-      <c r="G47" s="203"/>
-      <c r="H47" s="203"/>
-      <c r="I47" s="203"/>
-      <c r="J47" s="204"/>
+      <c r="A47" s="201"/>
+      <c r="B47" s="202"/>
+      <c r="C47" s="202"/>
+      <c r="D47" s="202"/>
+      <c r="E47" s="202"/>
+      <c r="F47" s="202"/>
+      <c r="G47" s="202"/>
+      <c r="H47" s="202"/>
+      <c r="I47" s="202"/>
+      <c r="J47" s="203"/>
     </row>
     <row r="48" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="193"/>
-      <c r="B48" s="194"/>
-      <c r="C48" s="194"/>
-      <c r="D48" s="194"/>
-      <c r="E48" s="194"/>
-      <c r="F48" s="194"/>
-      <c r="G48" s="194"/>
-      <c r="H48" s="194"/>
-      <c r="I48" s="194"/>
-      <c r="J48" s="195"/>
+      <c r="A48" s="204"/>
+      <c r="B48" s="205"/>
+      <c r="C48" s="205"/>
+      <c r="D48" s="205"/>
+      <c r="E48" s="205"/>
+      <c r="F48" s="205"/>
+      <c r="G48" s="205"/>
+      <c r="H48" s="205"/>
+      <c r="I48" s="205"/>
+      <c r="J48" s="206"/>
     </row>
     <row r="49" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="44"/>
@@ -3523,54 +3496,54 @@
       <c r="J50" s="46"/>
     </row>
     <row r="51" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="193"/>
-      <c r="B51" s="194"/>
-      <c r="C51" s="194"/>
-      <c r="D51" s="194"/>
-      <c r="E51" s="194"/>
-      <c r="F51" s="194"/>
-      <c r="G51" s="194"/>
-      <c r="H51" s="194"/>
-      <c r="I51" s="194"/>
-      <c r="J51" s="195"/>
+      <c r="A51" s="204"/>
+      <c r="B51" s="205"/>
+      <c r="C51" s="205"/>
+      <c r="D51" s="205"/>
+      <c r="E51" s="205"/>
+      <c r="F51" s="205"/>
+      <c r="G51" s="205"/>
+      <c r="H51" s="205"/>
+      <c r="I51" s="205"/>
+      <c r="J51" s="206"/>
     </row>
     <row r="52" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="193"/>
-      <c r="B52" s="194"/>
-      <c r="C52" s="194"/>
-      <c r="D52" s="194"/>
-      <c r="E52" s="194"/>
-      <c r="F52" s="194"/>
-      <c r="G52" s="194"/>
-      <c r="H52" s="194"/>
-      <c r="I52" s="194"/>
-      <c r="J52" s="195"/>
+      <c r="A52" s="204"/>
+      <c r="B52" s="205"/>
+      <c r="C52" s="205"/>
+      <c r="D52" s="205"/>
+      <c r="E52" s="205"/>
+      <c r="F52" s="205"/>
+      <c r="G52" s="205"/>
+      <c r="H52" s="205"/>
+      <c r="I52" s="205"/>
+      <c r="J52" s="206"/>
     </row>
     <row r="53" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="193" t="s">
+      <c r="A53" s="204" t="s">
         <v>60</v>
       </c>
-      <c r="B53" s="194"/>
-      <c r="C53" s="194"/>
-      <c r="D53" s="194"/>
-      <c r="E53" s="194"/>
-      <c r="F53" s="194"/>
-      <c r="G53" s="194"/>
-      <c r="H53" s="194"/>
-      <c r="I53" s="194"/>
-      <c r="J53" s="195"/>
+      <c r="B53" s="205"/>
+      <c r="C53" s="205"/>
+      <c r="D53" s="205"/>
+      <c r="E53" s="205"/>
+      <c r="F53" s="205"/>
+      <c r="G53" s="205"/>
+      <c r="H53" s="205"/>
+      <c r="I53" s="205"/>
+      <c r="J53" s="206"/>
     </row>
     <row r="54" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="205"/>
-      <c r="B54" s="206"/>
-      <c r="C54" s="206"/>
-      <c r="D54" s="206"/>
-      <c r="E54" s="206"/>
-      <c r="F54" s="206"/>
-      <c r="G54" s="206"/>
-      <c r="H54" s="206"/>
-      <c r="I54" s="206"/>
-      <c r="J54" s="207"/>
+      <c r="A54" s="207"/>
+      <c r="B54" s="208"/>
+      <c r="C54" s="208"/>
+      <c r="D54" s="208"/>
+      <c r="E54" s="208"/>
+      <c r="F54" s="208"/>
+      <c r="G54" s="208"/>
+      <c r="H54" s="208"/>
+      <c r="I54" s="208"/>
+      <c r="J54" s="209"/>
     </row>
     <row r="55" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="47"/>
@@ -3607,15 +3580,15 @@
       <c r="A58" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B58" s="208"/>
-      <c r="C58" s="209"/>
-      <c r="D58" s="209"/>
-      <c r="E58" s="209"/>
-      <c r="F58" s="209"/>
-      <c r="G58" s="209"/>
-      <c r="H58" s="209"/>
-      <c r="I58" s="209"/>
-      <c r="J58" s="210"/>
+      <c r="B58" s="210"/>
+      <c r="C58" s="211"/>
+      <c r="D58" s="211"/>
+      <c r="E58" s="211"/>
+      <c r="F58" s="211"/>
+      <c r="G58" s="211"/>
+      <c r="H58" s="211"/>
+      <c r="I58" s="211"/>
+      <c r="J58" s="212"/>
       <c r="K58" s="23"/>
     </row>
     <row r="59" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3788,64 +3761,64 @@
       <c r="I72" s="42"/>
     </row>
     <row r="73" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="202"/>
-      <c r="B73" s="203"/>
-      <c r="C73" s="203"/>
-      <c r="D73" s="203"/>
-      <c r="E73" s="203"/>
-      <c r="F73" s="203"/>
-      <c r="G73" s="203"/>
-      <c r="H73" s="203"/>
-      <c r="I73" s="203"/>
-      <c r="J73" s="204"/>
+      <c r="A73" s="201"/>
+      <c r="B73" s="202"/>
+      <c r="C73" s="202"/>
+      <c r="D73" s="202"/>
+      <c r="E73" s="202"/>
+      <c r="F73" s="202"/>
+      <c r="G73" s="202"/>
+      <c r="H73" s="202"/>
+      <c r="I73" s="202"/>
+      <c r="J73" s="203"/>
     </row>
     <row r="74" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="190"/>
-      <c r="B74" s="191"/>
-      <c r="C74" s="191"/>
-      <c r="D74" s="191"/>
-      <c r="E74" s="191"/>
-      <c r="F74" s="191"/>
-      <c r="G74" s="191"/>
-      <c r="H74" s="191"/>
-      <c r="I74" s="191"/>
-      <c r="J74" s="192"/>
+      <c r="A74" s="195"/>
+      <c r="B74" s="196"/>
+      <c r="C74" s="196"/>
+      <c r="D74" s="196"/>
+      <c r="E74" s="196"/>
+      <c r="F74" s="196"/>
+      <c r="G74" s="196"/>
+      <c r="H74" s="196"/>
+      <c r="I74" s="196"/>
+      <c r="J74" s="197"/>
     </row>
     <row r="75" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="190"/>
-      <c r="B75" s="191"/>
-      <c r="C75" s="191"/>
-      <c r="D75" s="191"/>
-      <c r="E75" s="191"/>
-      <c r="F75" s="191"/>
-      <c r="G75" s="191"/>
-      <c r="H75" s="191"/>
-      <c r="I75" s="191"/>
-      <c r="J75" s="192"/>
+      <c r="A75" s="195"/>
+      <c r="B75" s="196"/>
+      <c r="C75" s="196"/>
+      <c r="D75" s="196"/>
+      <c r="E75" s="196"/>
+      <c r="F75" s="196"/>
+      <c r="G75" s="196"/>
+      <c r="H75" s="196"/>
+      <c r="I75" s="196"/>
+      <c r="J75" s="197"/>
     </row>
     <row r="76" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="190"/>
-      <c r="B76" s="191"/>
-      <c r="C76" s="191"/>
-      <c r="D76" s="191"/>
-      <c r="E76" s="191"/>
-      <c r="F76" s="191"/>
-      <c r="G76" s="191"/>
-      <c r="H76" s="191"/>
-      <c r="I76" s="191"/>
-      <c r="J76" s="192"/>
+      <c r="A76" s="195"/>
+      <c r="B76" s="196"/>
+      <c r="C76" s="196"/>
+      <c r="D76" s="196"/>
+      <c r="E76" s="196"/>
+      <c r="F76" s="196"/>
+      <c r="G76" s="196"/>
+      <c r="H76" s="196"/>
+      <c r="I76" s="196"/>
+      <c r="J76" s="197"/>
     </row>
     <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="190"/>
-      <c r="B77" s="191"/>
-      <c r="C77" s="191"/>
-      <c r="D77" s="191"/>
-      <c r="E77" s="191"/>
-      <c r="F77" s="191"/>
-      <c r="G77" s="191"/>
-      <c r="H77" s="191"/>
-      <c r="I77" s="191"/>
-      <c r="J77" s="192"/>
+      <c r="A77" s="195"/>
+      <c r="B77" s="196"/>
+      <c r="C77" s="196"/>
+      <c r="D77" s="196"/>
+      <c r="E77" s="196"/>
+      <c r="F77" s="196"/>
+      <c r="G77" s="196"/>
+      <c r="H77" s="196"/>
+      <c r="I77" s="196"/>
+      <c r="J77" s="197"/>
     </row>
     <row r="78" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="54"/>
@@ -3860,30 +3833,30 @@
       <c r="J78" s="57"/>
     </row>
     <row r="79" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="193" t="s">
+      <c r="A79" s="204" t="s">
         <v>60</v>
       </c>
-      <c r="B79" s="194"/>
-      <c r="C79" s="194"/>
-      <c r="D79" s="194"/>
-      <c r="E79" s="194"/>
-      <c r="F79" s="194"/>
-      <c r="G79" s="194"/>
-      <c r="H79" s="194"/>
-      <c r="I79" s="194"/>
-      <c r="J79" s="195"/>
+      <c r="B79" s="205"/>
+      <c r="C79" s="205"/>
+      <c r="D79" s="205"/>
+      <c r="E79" s="205"/>
+      <c r="F79" s="205"/>
+      <c r="G79" s="205"/>
+      <c r="H79" s="205"/>
+      <c r="I79" s="205"/>
+      <c r="J79" s="206"/>
     </row>
     <row r="80" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="196"/>
-      <c r="B80" s="197"/>
-      <c r="C80" s="197"/>
-      <c r="D80" s="197"/>
-      <c r="E80" s="197"/>
-      <c r="F80" s="197"/>
-      <c r="G80" s="197"/>
-      <c r="H80" s="197"/>
-      <c r="I80" s="197"/>
-      <c r="J80" s="198"/>
+      <c r="A80" s="213"/>
+      <c r="B80" s="214"/>
+      <c r="C80" s="214"/>
+      <c r="D80" s="214"/>
+      <c r="E80" s="214"/>
+      <c r="F80" s="214"/>
+      <c r="G80" s="214"/>
+      <c r="H80" s="214"/>
+      <c r="I80" s="214"/>
+      <c r="J80" s="215"/>
     </row>
     <row r="81" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C81" s="42"/>
@@ -3918,7 +3891,7 @@
         <v>74</v>
       </c>
       <c r="B85" s="58" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C85" s="58"/>
       <c r="D85" s="58"/>
@@ -3944,8 +3917,8 @@
       <c r="A87" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="B87" s="182" t="s">
-        <v>264</v>
+      <c r="B87" s="181" t="s">
+        <v>263</v>
       </c>
       <c r="C87" s="59"/>
       <c r="D87" s="59"/>
@@ -6026,14 +5999,11 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="A75:J75"/>
+    <mergeCell ref="A76:J76"/>
+    <mergeCell ref="A77:J77"/>
+    <mergeCell ref="A79:J79"/>
+    <mergeCell ref="A80:J80"/>
     <mergeCell ref="A74:J74"/>
     <mergeCell ref="J16:J17"/>
     <mergeCell ref="K16:K17"/>
@@ -6046,11 +6016,14 @@
     <mergeCell ref="A54:J54"/>
     <mergeCell ref="B58:J58"/>
     <mergeCell ref="A73:J73"/>
-    <mergeCell ref="A75:J75"/>
-    <mergeCell ref="A76:J76"/>
-    <mergeCell ref="A77:J77"/>
-    <mergeCell ref="A79:J79"/>
-    <mergeCell ref="A80:J80"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6061,7 +6034,7 @@
   <dimension ref="A1:L376"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="A26" sqref="A26:J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6077,18 +6050,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="184"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="237" t="s">
         <v>266</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="187"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="188" t="s">
-        <v>267</v>
-      </c>
       <c r="I2" s="3"/>
-      <c r="J2" s="189"/>
+      <c r="J2" s="185"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I3" s="3"/>
@@ -6122,10 +6095,10 @@
     </row>
     <row r="6" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="B6" s="246" t="s">
-        <v>268</v>
+        <v>264</v>
+      </c>
+      <c r="B6" s="247" t="s">
+        <v>267</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -6142,8 +6115,8 @@
       <c r="A7" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="185" t="s">
-        <v>259</v>
+      <c r="B7" s="248" t="s">
+        <v>258</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
@@ -6158,7 +6131,7 @@
       <c r="A8" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="246" t="s">
         <v>79</v>
       </c>
       <c r="C8" s="15"/>
@@ -6174,8 +6147,8 @@
       <c r="A9" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="185" t="s">
-        <v>260</v>
+      <c r="B9" s="248" t="s">
+        <v>259</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
@@ -6184,7 +6157,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
-      <c r="J9" s="183" t="s">
+      <c r="J9" s="182" t="s">
         <v>269</v>
       </c>
     </row>
@@ -6202,7 +6175,7 @@
       <c r="G10" s="14"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
-      <c r="J10" s="184" t="s">
+      <c r="J10" s="183" t="s">
         <v>270</v>
       </c>
     </row>
@@ -6219,35 +6192,35 @@
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="236" t="s">
+      <c r="A12" s="218" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="238" t="s">
+      <c r="B12" s="220" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="240" t="s">
+      <c r="C12" s="222" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="229" t="s">
+      <c r="D12" s="224" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="230"/>
-      <c r="F12" s="231"/>
-      <c r="G12" s="229" t="s">
+      <c r="E12" s="225"/>
+      <c r="F12" s="226"/>
+      <c r="G12" s="224" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="230"/>
-      <c r="I12" s="231"/>
-      <c r="J12" s="232" t="s">
+      <c r="H12" s="225"/>
+      <c r="I12" s="226"/>
+      <c r="J12" s="231" t="s">
         <v>10</v>
       </c>
-      <c r="K12" s="201"/>
-      <c r="L12" s="201"/>
+      <c r="K12" s="200"/>
+      <c r="L12" s="200"/>
     </row>
     <row r="13" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="237"/>
-      <c r="B13" s="239"/>
-      <c r="C13" s="241"/>
+      <c r="A13" s="219"/>
+      <c r="B13" s="221"/>
+      <c r="C13" s="223"/>
       <c r="D13" s="65" t="s">
         <v>11</v>
       </c>
@@ -6266,23 +6239,23 @@
       <c r="I13" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="233"/>
-      <c r="K13" s="201"/>
-      <c r="L13" s="201"/>
+      <c r="J13" s="232"/>
+      <c r="K13" s="200"/>
+      <c r="L13" s="200"/>
     </row>
     <row r="14" spans="1:12" s="66" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="225" t="s">
+      <c r="A14" s="227" t="s">
         <v>83</v>
       </c>
-      <c r="B14" s="225"/>
-      <c r="C14" s="225"/>
-      <c r="D14" s="225"/>
-      <c r="E14" s="225"/>
-      <c r="F14" s="225"/>
-      <c r="G14" s="225"/>
-      <c r="H14" s="225"/>
-      <c r="I14" s="225"/>
-      <c r="J14" s="225"/>
+      <c r="B14" s="227"/>
+      <c r="C14" s="227"/>
+      <c r="D14" s="227"/>
+      <c r="E14" s="227"/>
+      <c r="F14" s="227"/>
+      <c r="G14" s="227"/>
+      <c r="H14" s="227"/>
+      <c r="I14" s="227"/>
+      <c r="J14" s="227"/>
     </row>
     <row r="15" spans="1:12" s="71" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="67" t="s">
@@ -6523,18 +6496,18 @@
       <c r="J25" s="78"/>
     </row>
     <row r="26" spans="1:10" s="71" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="226" t="s">
+      <c r="A26" s="228" t="s">
         <v>100</v>
       </c>
-      <c r="B26" s="226"/>
-      <c r="C26" s="226"/>
-      <c r="D26" s="226"/>
-      <c r="E26" s="226"/>
-      <c r="F26" s="226"/>
-      <c r="G26" s="226"/>
-      <c r="H26" s="226"/>
-      <c r="I26" s="226"/>
-      <c r="J26" s="226"/>
+      <c r="B26" s="228"/>
+      <c r="C26" s="228"/>
+      <c r="D26" s="228"/>
+      <c r="E26" s="228"/>
+      <c r="F26" s="228"/>
+      <c r="G26" s="228"/>
+      <c r="H26" s="228"/>
+      <c r="I26" s="228"/>
+      <c r="J26" s="228"/>
     </row>
     <row r="27" spans="1:10" s="71" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="67" t="s">
@@ -7743,10 +7716,10 @@
       <c r="J88" s="28"/>
     </row>
     <row r="89" spans="1:10" s="29" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="227" t="s">
+      <c r="A89" s="229" t="s">
         <v>204</v>
       </c>
-      <c r="B89" s="228"/>
+      <c r="B89" s="230"/>
       <c r="C89" s="149"/>
       <c r="D89" s="150"/>
       <c r="E89" s="150"/>
@@ -7757,14 +7730,14 @@
       <c r="J89" s="126"/>
     </row>
     <row r="90" spans="1:10" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="234" t="s">
+      <c r="A90" s="216" t="s">
         <v>205</v>
       </c>
-      <c r="B90" s="234"/>
-      <c r="C90" s="234"/>
-      <c r="D90" s="234"/>
-      <c r="E90" s="234"/>
-      <c r="F90" s="235"/>
+      <c r="B90" s="216"/>
+      <c r="C90" s="216"/>
+      <c r="D90" s="216"/>
+      <c r="E90" s="216"/>
+      <c r="F90" s="217"/>
       <c r="G90" s="30" t="s">
         <v>19</v>
       </c>
@@ -9335,11 +9308,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A90:F90"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:F12"/>
     <mergeCell ref="K12:K13"/>
     <mergeCell ref="L12:L13"/>
     <mergeCell ref="A14:J14"/>
@@ -9347,6 +9315,11 @@
     <mergeCell ref="A89:B89"/>
     <mergeCell ref="G12:I12"/>
     <mergeCell ref="J12:J13"/>
+    <mergeCell ref="A90:F90"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9357,7 +9330,7 @@
   <dimension ref="A1:J291"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9375,20 +9348,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="186" t="s">
-        <v>266</v>
+      <c r="A1" s="17" t="s">
+        <v>265</v>
       </c>
       <c r="G1" s="1"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="187"/>
+      <c r="J1" s="184"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="188" t="s">
-        <v>267</v>
+      <c r="A2" s="237" t="s">
+        <v>266</v>
       </c>
       <c r="G2" s="1"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="189"/>
+      <c r="J2" s="185"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I3" s="3"/>
@@ -9610,11 +9583,11 @@
       <c r="B17" s="76"/>
       <c r="C17" s="75"/>
       <c r="D17" s="75"/>
-      <c r="E17" s="242" t="s">
+      <c r="E17" s="233" t="s">
         <v>237</v>
       </c>
-      <c r="F17" s="242"/>
-      <c r="G17" s="242"/>
+      <c r="F17" s="233"/>
+      <c r="G17" s="233"/>
       <c r="H17" s="173"/>
       <c r="I17" s="75"/>
       <c r="J17" s="75" t="s">
@@ -9774,19 +9747,19 @@
       <c r="J27" s="60"/>
     </row>
     <row r="28" spans="1:10" s="73" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="243" t="s">
+      <c r="A28" s="234" t="s">
         <v>245</v>
       </c>
-      <c r="B28" s="243"/>
+      <c r="B28" s="234"/>
       <c r="C28" s="175" t="s">
         <v>246</v>
       </c>
-      <c r="D28" s="243" t="s">
+      <c r="D28" s="234" t="s">
         <v>247</v>
       </c>
-      <c r="E28" s="243"/>
-      <c r="F28" s="243"/>
-      <c r="G28" s="243"/>
+      <c r="E28" s="234"/>
+      <c r="F28" s="234"/>
+      <c r="G28" s="234"/>
       <c r="I28" s="176" t="s">
         <v>246</v>
       </c>
@@ -9795,16 +9768,16 @@
       </c>
     </row>
     <row r="29" spans="1:10" s="73" customFormat="1" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="244" t="s">
+      <c r="A29" s="235" t="s">
         <v>248</v>
       </c>
-      <c r="B29" s="244"/>
-      <c r="D29" s="245">
+      <c r="B29" s="235"/>
+      <c r="D29" s="236">
         <v>113.8</v>
       </c>
-      <c r="E29" s="245"/>
-      <c r="F29" s="245"/>
-      <c r="G29" s="245"/>
+      <c r="E29" s="236"/>
+      <c r="F29" s="236"/>
+      <c r="G29" s="236"/>
     </row>
     <row r="30" spans="1:10" s="29" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="60"/>

</xml_diff>